<commit_message>
More experiments with Autoformat
</commit_message>
<xml_diff>
--- a/AutoFormatExperiment.xlsx
+++ b/AutoFormatExperiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2E85F13-80F6-4DE6-9B6D-0DD20DBE9A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{A2E85F13-80F6-4DE6-9B6D-0DD20DBE9A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DE5D1A4-5911-4EB4-8893-8CA283FFB74D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>FROM:</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>Row 5</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Row 6</t>
+  </si>
+  <si>
+    <t>Row 7</t>
+  </si>
+  <si>
+    <t>Future Tasks</t>
+  </si>
+  <si>
+    <t>Macro to format the data</t>
   </si>
 </sst>
 </file>
@@ -86,7 +101,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -224,8 +239,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +310,26 @@
         <bgColor indexed="24"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="darkGray">
+        <fgColor indexed="9"/>
+        <bgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="15"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -368,6 +428,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -385,7 +454,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -423,6 +492,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -755,23 +843,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="4" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="28" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,14 +870,17 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AE2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -812,8 +905,11 @@
       <c r="AB3" s="18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AE3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="W4" s="16" t="s">
         <v>9</v>
       </c>
@@ -830,11 +926,11 @@
         <v>91</v>
       </c>
       <c r="AB4" s="15">
-        <f>SUM(X4:AA4)</f>
+        <f t="shared" ref="AB4:AB9" si="0">SUM(X4:AA4)</f>
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="W5" s="16" t="s">
         <v>10</v>
       </c>
@@ -851,11 +947,11 @@
         <v>50</v>
       </c>
       <c r="AB5" s="15">
-        <f>SUM(X5:AA5)</f>
+        <f t="shared" si="0"/>
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="W6" s="17" t="s">
         <v>11</v>
       </c>
@@ -872,11 +968,11 @@
         <v>64</v>
       </c>
       <c r="AB6" s="13">
-        <f>SUM(X6:AA6)</f>
+        <f t="shared" si="0"/>
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="W7" s="17" t="s">
         <v>12</v>
       </c>
@@ -893,11 +989,11 @@
         <v>22</v>
       </c>
       <c r="AB7" s="13">
-        <f>SUM(X7:AA7)</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="W8" s="16" t="s">
         <v>13</v>
       </c>
@@ -914,11 +1010,11 @@
         <v>48</v>
       </c>
       <c r="AB8" s="15">
-        <f>SUM(X8:AA8)</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -963,11 +1059,11 @@
         <v>275</v>
       </c>
       <c r="AB9" s="20">
-        <f>SUM(X9:AA9)</f>
+        <f t="shared" si="0"/>
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>39</v>
       </c>
@@ -993,7 +1089,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>14</v>
       </c>
@@ -1019,7 +1115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>55</v>
       </c>
@@ -1045,7 +1141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>16</v>
       </c>
@@ -1071,7 +1167,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>41</v>
       </c>
@@ -1096,8 +1192,47 @@
       <c r="N14" s="5">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="X14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z14" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB14" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15" s="15">
+        <v>39</v>
+      </c>
+      <c r="Y15" s="15">
+        <v>79</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>23</v>
+      </c>
+      <c r="AA15" s="15">
+        <v>91</v>
+      </c>
+      <c r="AB15" s="15">
+        <f>SUM(X15:AA15)</f>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P16" s="9" t="s">
         <v>4</v>
       </c>
@@ -1110,8 +1245,27 @@
       <c r="S16" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="X16" s="15">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="15">
+        <v>24</v>
+      </c>
+      <c r="Z16" s="15">
+        <v>94</v>
+      </c>
+      <c r="AA16" s="15">
+        <v>50</v>
+      </c>
+      <c r="AB16" s="15">
+        <f>SUM(X16:AA16)</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P17" s="7">
         <v>39</v>
       </c>
@@ -1124,8 +1278,27 @@
       <c r="S17" s="7">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="X17" s="13">
+        <v>55</v>
+      </c>
+      <c r="Y17" s="13">
+        <v>35</v>
+      </c>
+      <c r="Z17" s="13">
+        <v>57</v>
+      </c>
+      <c r="AA17" s="13">
+        <v>64</v>
+      </c>
+      <c r="AB17" s="13">
+        <f>SUM(X17:AA17)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P18" s="8">
         <v>14</v>
       </c>
@@ -1138,8 +1311,27 @@
       <c r="S18" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="X18" s="13">
+        <v>16</v>
+      </c>
+      <c r="Y18" s="13">
+        <v>29</v>
+      </c>
+      <c r="Z18" s="13">
+        <v>9</v>
+      </c>
+      <c r="AA18" s="13">
+        <v>22</v>
+      </c>
+      <c r="AB18" s="13">
+        <f>SUM(X18:AA18)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P19" s="8">
         <v>55</v>
       </c>
@@ -1152,8 +1344,27 @@
       <c r="S19" s="8">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W19" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="X19" s="15">
+        <v>41</v>
+      </c>
+      <c r="Y19" s="15">
+        <v>14</v>
+      </c>
+      <c r="Z19" s="15">
+        <v>37</v>
+      </c>
+      <c r="AA19" s="15">
+        <v>48</v>
+      </c>
+      <c r="AB19" s="15">
+        <f>SUM(X19:AA19)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P20" s="8">
         <v>16</v>
       </c>
@@ -1166,8 +1377,27 @@
       <c r="S20" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X20" s="15">
+        <v>55</v>
+      </c>
+      <c r="Y20" s="15">
+        <v>35</v>
+      </c>
+      <c r="Z20" s="15">
+        <v>57</v>
+      </c>
+      <c r="AA20" s="15">
+        <v>64</v>
+      </c>
+      <c r="AB20" s="15">
+        <f>SUM(X20:AA20)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P21" s="8">
         <v>41</v>
       </c>
@@ -1180,9 +1410,53 @@
       <c r="S21" s="8">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="16:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="16:20" x14ac:dyDescent="0.2">
+      <c r="W21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="X21" s="13">
+        <v>16</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>29</v>
+      </c>
+      <c r="Z21" s="13">
+        <v>9</v>
+      </c>
+      <c r="AA21" s="13">
+        <v>22</v>
+      </c>
+      <c r="AB21" s="13">
+        <f>SUM(X21:AA21)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W22" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="X22" s="20">
+        <f>SUM(X15:X21)</f>
+        <v>236</v>
+      </c>
+      <c r="Y22" s="20">
+        <f>SUM(Y15:Y21)</f>
+        <v>245</v>
+      </c>
+      <c r="Z22" s="20">
+        <f>SUM(Z15:Z21)</f>
+        <v>286</v>
+      </c>
+      <c r="AA22" s="20">
+        <f>SUM(AA15:AA21)</f>
+        <v>361</v>
+      </c>
+      <c r="AB22" s="20">
+        <f>SUM(X22:AA22)</f>
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P24" s="10" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="16:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P25" s="3">
         <v>39</v>
       </c>
@@ -1213,11 +1487,11 @@
         <v>91</v>
       </c>
       <c r="T25" s="3">
-        <f>SUM(P25:S25)</f>
+        <f t="shared" ref="T25:T30" si="1">SUM(P25:S25)</f>
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="16:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.2">
       <c r="P26" s="3">
         <v>14</v>
       </c>
@@ -1231,11 +1505,29 @@
         <v>50</v>
       </c>
       <c r="T26" s="3">
-        <f>SUM(P26:S26)</f>
+        <f t="shared" si="1"/>
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="16:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="P27" s="3">
         <v>55</v>
       </c>
@@ -1249,11 +1541,30 @@
         <v>64</v>
       </c>
       <c r="T27" s="3">
-        <f>SUM(P27:S27)</f>
+        <f t="shared" si="1"/>
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="16:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B28" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="21">
+        <v>39</v>
+      </c>
+      <c r="D28" s="21">
+        <v>79</v>
+      </c>
+      <c r="E28" s="21">
+        <v>23</v>
+      </c>
+      <c r="F28" s="21">
+        <v>91</v>
+      </c>
+      <c r="G28" s="27">
+        <f>SUM(C28:F28)</f>
+        <v>232</v>
+      </c>
       <c r="P28" s="3">
         <v>16</v>
       </c>
@@ -1267,11 +1578,30 @@
         <v>22</v>
       </c>
       <c r="T28" s="3">
-        <f>SUM(P28:S28)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="16:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="21">
+        <v>14</v>
+      </c>
+      <c r="D29" s="21">
+        <v>24</v>
+      </c>
+      <c r="E29" s="21">
+        <v>94</v>
+      </c>
+      <c r="F29" s="21">
+        <v>50</v>
+      </c>
+      <c r="G29" s="27">
+        <f>SUM(C29:F29)</f>
+        <v>182</v>
+      </c>
       <c r="P29" s="3">
         <v>41</v>
       </c>
@@ -1285,11 +1615,30 @@
         <v>48</v>
       </c>
       <c r="T29" s="3">
-        <f>SUM(P29:S29)</f>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="16:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="21">
+        <v>55</v>
+      </c>
+      <c r="D30" s="21">
+        <v>35</v>
+      </c>
+      <c r="E30" s="21">
+        <v>57</v>
+      </c>
+      <c r="F30" s="21">
+        <v>64</v>
+      </c>
+      <c r="G30" s="27">
+        <f>SUM(C30:F30)</f>
+        <v>211</v>
+      </c>
       <c r="P30" s="12">
         <f>SUM(P25:P29)</f>
         <v>165</v>
@@ -1307,7 +1656,74 @@
         <v>275</v>
       </c>
       <c r="T30" s="12">
-        <f>SUM(P30:S30)</f>
+        <f t="shared" si="1"/>
+        <v>841</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B31" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="21">
+        <v>16</v>
+      </c>
+      <c r="D31" s="21">
+        <v>29</v>
+      </c>
+      <c r="E31" s="21">
+        <v>9</v>
+      </c>
+      <c r="F31" s="21">
+        <v>22</v>
+      </c>
+      <c r="G31" s="27">
+        <f>SUM(C31:F31)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B32" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="21">
+        <v>41</v>
+      </c>
+      <c r="D32" s="21">
+        <v>14</v>
+      </c>
+      <c r="E32" s="21">
+        <v>37</v>
+      </c>
+      <c r="F32" s="21">
+        <v>48</v>
+      </c>
+      <c r="G32" s="27">
+        <f>SUM(C32:F32)</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="24">
+        <f>SUM(C28:C32)</f>
+        <v>165</v>
+      </c>
+      <c r="D33" s="24">
+        <f>SUM(D28:D32)</f>
+        <v>181</v>
+      </c>
+      <c r="E33" s="24">
+        <f>SUM(E28:E32)</f>
+        <v>220</v>
+      </c>
+      <c r="F33" s="24">
+        <f>SUM(F28:F32)</f>
+        <v>275</v>
+      </c>
+      <c r="G33" s="28">
+        <f>SUM(C33:F33)</f>
         <v>841</v>
       </c>
     </row>

</xml_diff>